<commit_message>
final tweaks to readme, add another image, add title to excel chart
</commit_message>
<xml_diff>
--- a/results/GA Output - Circularity 01.xlsx
+++ b/results/GA Output - Circularity 01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\James\Code\Javascript\Decode Drawings V5\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C58D42B-B3E0-40F0-B498-75F1B1CB7D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BF577E-DA99-4C8A-8792-7194786C1A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1C324745-2B40-4F8F-A1A3-999737C74E32}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1C324745-2B40-4F8F-A1A3-999737C74E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,6 +128,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Circle Error over 50k generations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21241,6 +21266,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="352134351"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -22223,7 +22249,7 @@
   <dimension ref="A1:Q431"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>